<commit_message>
Update data from gsheets
</commit_message>
<xml_diff>
--- a/scripts/tests/input/MARCO-BOLO_Metadata_Dataset_Record_WP2.xlsx
+++ b/scripts/tests/input/MARCO-BOLO_Metadata_Dataset_Record_WP2.xlsx
@@ -11,14 +11,14 @@
   <calcPr/>
   <extLst>
     <ext uri="GoogleSheetsCustomDataVersion2">
-      <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="rId7" roundtripDataChecksum="4cK8omZTn4xBUi/cgo3PjHiAflOiKXv0KoCePQfUzRA="/>
+      <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="rId7" roundtripDataChecksum="eaS7mkUaUIyCk7PAtv7P8yCtJ0225qM6Dk8T9MCgpc4="/>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="227" uniqueCount="136">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="224" uniqueCount="135">
   <si>
     <t>Sheet Name</t>
   </si>
@@ -361,9 +361,6 @@
     <t>2024-12-01</t>
   </si>
   <si>
-    <t>N/A</t>
-  </si>
-  <si>
     <t>Task2.1_sourceData2</t>
   </si>
   <si>
@@ -543,7 +540,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="42">
+  <cellXfs count="43">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -641,6 +638,9 @@
     </xf>
     <xf borderId="0" fillId="0" fontId="6" numFmtId="164" xfId="0" applyFont="1" applyNumberFormat="1"/>
     <xf borderId="0" fillId="0" fontId="6" numFmtId="49" xfId="0" applyFont="1" applyNumberFormat="1"/>
+    <xf borderId="0" fillId="0" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0"/>
+    </xf>
     <xf borderId="1" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center" shrinkToFit="0" wrapText="1"/>
     </xf>
@@ -5325,8 +5325,8 @@
     </row>
   </sheetData>
   <mergeCells count="2">
+    <mergeCell ref="A2:A29"/>
     <mergeCell ref="A30:A37"/>
-    <mergeCell ref="A2:A29"/>
   </mergeCells>
   <printOptions/>
   <pageMargins bottom="0.75" footer="0.0" header="0.0" left="0.7" right="0.7" top="0.75"/>
@@ -5453,183 +5453,203 @@
       <c r="G2" s="34" t="s">
         <v>110</v>
       </c>
-      <c r="H2" s="28" t="s">
-        <v>111</v>
-      </c>
+      <c r="H2" s="28"/>
       <c r="U2" s="35"/>
       <c r="V2" s="35"/>
     </row>
     <row r="3" ht="14.25" customHeight="1">
       <c r="A3" s="28" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="B3" s="28" t="s">
         <v>107</v>
       </c>
       <c r="C3" s="28" t="s">
+        <v>112</v>
+      </c>
+      <c r="D3" s="28" t="s">
         <v>113</v>
-      </c>
-      <c r="D3" s="28" t="s">
-        <v>114</v>
       </c>
       <c r="G3" s="34" t="s">
         <v>110</v>
       </c>
-      <c r="H3" s="28" t="s">
-        <v>111</v>
-      </c>
+      <c r="H3" s="28"/>
       <c r="U3" s="35"/>
       <c r="V3" s="35"/>
     </row>
     <row r="4" ht="14.25" customHeight="1">
       <c r="A4" s="28" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="B4" s="28" t="s">
         <v>107</v>
       </c>
       <c r="C4" s="28" t="s">
+        <v>115</v>
+      </c>
+      <c r="D4" s="28" t="s">
         <v>116</v>
-      </c>
-      <c r="D4" s="28" t="s">
-        <v>117</v>
       </c>
       <c r="G4" s="34" t="s">
         <v>110</v>
       </c>
-      <c r="H4" s="28" t="s">
-        <v>111</v>
-      </c>
+      <c r="H4" s="28"/>
       <c r="U4" s="35"/>
       <c r="V4" s="35"/>
     </row>
     <row r="5" ht="14.25" customHeight="1">
       <c r="G5" s="36"/>
+      <c r="H5" s="37"/>
       <c r="U5" s="35"/>
       <c r="V5" s="35"/>
     </row>
     <row r="6" ht="14.25" customHeight="1">
       <c r="G6" s="36"/>
+      <c r="H6" s="37"/>
       <c r="U6" s="35"/>
       <c r="V6" s="35"/>
     </row>
     <row r="7" ht="14.25" customHeight="1">
       <c r="G7" s="36"/>
+      <c r="H7" s="37"/>
       <c r="U7" s="35"/>
       <c r="V7" s="35"/>
     </row>
     <row r="8" ht="14.25" customHeight="1">
       <c r="G8" s="36"/>
+      <c r="H8" s="37"/>
       <c r="U8" s="35"/>
       <c r="V8" s="35"/>
     </row>
     <row r="9" ht="14.25" customHeight="1">
       <c r="G9" s="36"/>
+      <c r="H9" s="37"/>
       <c r="U9" s="35"/>
       <c r="V9" s="35"/>
     </row>
     <row r="10" ht="14.25" customHeight="1">
       <c r="G10" s="36"/>
+      <c r="H10" s="37"/>
       <c r="U10" s="35"/>
       <c r="V10" s="35"/>
     </row>
     <row r="11" ht="14.25" customHeight="1">
       <c r="G11" s="36"/>
+      <c r="H11" s="28"/>
       <c r="U11" s="35"/>
       <c r="V11" s="35"/>
     </row>
     <row r="12" ht="14.25" customHeight="1">
       <c r="G12" s="36"/>
+      <c r="H12" s="28"/>
       <c r="U12" s="35"/>
       <c r="V12" s="35"/>
     </row>
     <row r="13" ht="14.25" customHeight="1">
       <c r="G13" s="36"/>
+      <c r="H13" s="28"/>
       <c r="U13" s="35"/>
       <c r="V13" s="35"/>
     </row>
     <row r="14" ht="14.25" customHeight="1">
       <c r="G14" s="36"/>
+      <c r="H14" s="37"/>
       <c r="U14" s="35"/>
       <c r="V14" s="35"/>
     </row>
     <row r="15" ht="14.25" customHeight="1">
       <c r="G15" s="36"/>
+      <c r="H15" s="37"/>
       <c r="U15" s="35"/>
       <c r="V15" s="35"/>
     </row>
     <row r="16" ht="14.25" customHeight="1">
       <c r="G16" s="36"/>
+      <c r="H16" s="28"/>
       <c r="U16" s="35"/>
       <c r="V16" s="35"/>
     </row>
     <row r="17" ht="14.25" customHeight="1">
       <c r="G17" s="36"/>
+      <c r="H17" s="28"/>
       <c r="U17" s="35"/>
       <c r="V17" s="35"/>
     </row>
     <row r="18" ht="14.25" customHeight="1">
       <c r="G18" s="36"/>
+      <c r="H18" s="28"/>
       <c r="U18" s="35"/>
       <c r="V18" s="35"/>
     </row>
     <row r="19" ht="14.25" customHeight="1">
       <c r="G19" s="36"/>
+      <c r="H19" s="37"/>
       <c r="U19" s="35"/>
       <c r="V19" s="35"/>
     </row>
     <row r="20" ht="14.25" customHeight="1">
       <c r="G20" s="36"/>
+      <c r="H20" s="37"/>
       <c r="U20" s="35"/>
       <c r="V20" s="35"/>
     </row>
     <row r="21" ht="14.25" customHeight="1">
       <c r="G21" s="36"/>
+      <c r="H21" s="28"/>
       <c r="U21" s="35"/>
       <c r="V21" s="35"/>
     </row>
     <row r="22" ht="14.25" customHeight="1">
       <c r="G22" s="36"/>
+      <c r="H22" s="28"/>
       <c r="U22" s="35"/>
       <c r="V22" s="35"/>
     </row>
     <row r="23" ht="14.25" customHeight="1">
       <c r="G23" s="36"/>
+      <c r="H23" s="28"/>
       <c r="U23" s="35"/>
       <c r="V23" s="35"/>
     </row>
     <row r="24" ht="14.25" customHeight="1">
       <c r="G24" s="36"/>
+      <c r="H24" s="37"/>
       <c r="U24" s="35"/>
       <c r="V24" s="35"/>
     </row>
     <row r="25" ht="14.25" customHeight="1">
       <c r="G25" s="36"/>
+      <c r="H25" s="37"/>
       <c r="U25" s="35"/>
       <c r="V25" s="35"/>
     </row>
     <row r="26" ht="14.25" customHeight="1">
       <c r="G26" s="36"/>
+      <c r="H26" s="28"/>
       <c r="U26" s="35"/>
       <c r="V26" s="35"/>
     </row>
     <row r="27" ht="14.25" customHeight="1">
       <c r="G27" s="36"/>
+      <c r="H27" s="28"/>
       <c r="U27" s="35"/>
       <c r="V27" s="35"/>
     </row>
     <row r="28" ht="14.25" customHeight="1">
       <c r="G28" s="36"/>
+      <c r="H28" s="28"/>
       <c r="U28" s="35"/>
       <c r="V28" s="35"/>
     </row>
     <row r="29" ht="14.25" customHeight="1">
       <c r="G29" s="36"/>
+      <c r="H29" s="37"/>
       <c r="U29" s="35"/>
       <c r="V29" s="35"/>
     </row>
     <row r="30" ht="14.25" customHeight="1">
       <c r="G30" s="36"/>
+      <c r="H30" s="37"/>
       <c r="U30" s="35"/>
       <c r="V30" s="35"/>
     </row>
@@ -10469,6 +10489,11 @@
       <c r="V997" s="35"/>
     </row>
   </sheetData>
+  <dataValidations>
+    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="H2:H30">
+      <formula1>"Phytoplankton biomass and diversity,Zooplankton biomass and diversity,Fish abundance and distribution,Marine turtles, birds, mammals abundance and distribution,Hard coral cover and composition,Seagrass cover and composition,Macroalgal canopy cover and com"&amp;"position,Mangrove cover and composition"</formula1>
+    </dataValidation>
+  </dataValidations>
   <printOptions/>
   <pageMargins bottom="0.75" footer="0.0" header="0.0" left="0.7" right="0.7" top="0.75"/>
   <pageSetup orientation="landscape"/>
@@ -10489,65 +10514,65 @@
   </sheetViews>
   <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.0"/>
   <cols>
-    <col customWidth="1" min="1" max="1" width="9.43"/>
-    <col customWidth="1" min="2" max="2" width="11.86"/>
-    <col customWidth="1" min="3" max="3" width="37.14"/>
-    <col customWidth="1" min="4" max="4" width="23.0"/>
-    <col customWidth="1" min="5" max="5" width="18.43"/>
-    <col customWidth="1" min="6" max="6" width="52.29"/>
-    <col customWidth="1" min="7" max="7" width="26.14"/>
-    <col customWidth="1" min="8" max="8" width="9.86"/>
+    <col customWidth="1" min="1" max="1" width="9.57"/>
+    <col customWidth="1" min="2" max="2" width="17.57"/>
+    <col customWidth="1" min="3" max="3" width="35.0"/>
+    <col customWidth="1" min="4" max="4" width="51.14"/>
+    <col customWidth="1" min="5" max="5" width="18.14"/>
+    <col customWidth="1" min="6" max="6" width="64.0"/>
+    <col customWidth="1" min="7" max="7" width="24.71"/>
+    <col customWidth="1" min="8" max="8" width="8.14"/>
     <col customWidth="1" min="9" max="26" width="19.57"/>
   </cols>
   <sheetData>
     <row r="1" ht="14.25" customHeight="1">
-      <c r="A1" s="37" t="s">
+      <c r="A1" s="38" t="s">
         <v>86</v>
       </c>
-      <c r="B1" s="37" t="s">
+      <c r="B1" s="38" t="s">
         <v>88</v>
       </c>
-      <c r="C1" s="37" t="s">
+      <c r="C1" s="38" t="s">
         <v>91</v>
       </c>
-      <c r="D1" s="37" t="s">
+      <c r="D1" s="38" t="s">
         <v>93</v>
       </c>
-      <c r="E1" s="37" t="s">
+      <c r="E1" s="38" t="s">
         <v>95</v>
       </c>
-      <c r="F1" s="37" t="s">
+      <c r="F1" s="38" t="s">
         <v>97</v>
       </c>
-      <c r="G1" s="37" t="s">
+      <c r="G1" s="38" t="s">
         <v>99</v>
       </c>
-      <c r="H1" s="37" t="s">
+      <c r="H1" s="38" t="s">
         <v>102</v>
       </c>
     </row>
     <row r="2" ht="14.25" customHeight="1">
-      <c r="A2" s="38" t="s">
+      <c r="A2" s="39" t="s">
+        <v>117</v>
+      </c>
+      <c r="B2" s="39" t="s">
         <v>118</v>
       </c>
-      <c r="B2" s="38" t="s">
+      <c r="C2" s="39" t="s">
         <v>119</v>
       </c>
-      <c r="C2" s="38" t="s">
+      <c r="D2" s="39" t="s">
         <v>120</v>
       </c>
-      <c r="D2" s="38" t="s">
+      <c r="E2" s="39"/>
+      <c r="F2" s="10" t="s">
         <v>121</v>
       </c>
-      <c r="E2" s="38"/>
-      <c r="F2" s="10" t="s">
+      <c r="G2" s="39" t="s">
         <v>122</v>
       </c>
-      <c r="G2" s="38" t="s">
+      <c r="H2" s="39" t="s">
         <v>123</v>
-      </c>
-      <c r="H2" s="38" t="s">
-        <v>124</v>
       </c>
       <c r="I2" s="10"/>
       <c r="J2" s="10"/>
@@ -10573,45 +10598,45 @@
         <v>107</v>
       </c>
       <c r="B3" s="28" t="s">
+        <v>124</v>
+      </c>
+      <c r="C3" s="40" t="s">
         <v>125</v>
       </c>
-      <c r="C3" s="39" t="s">
+      <c r="D3" s="28" t="s">
         <v>126</v>
       </c>
-      <c r="D3" s="28" t="s">
+      <c r="E3" s="28" t="s">
         <v>127</v>
       </c>
-      <c r="E3" s="28" t="s">
+      <c r="G3" s="28" t="s">
         <v>128</v>
       </c>
-      <c r="G3" s="28" t="s">
+      <c r="H3" s="28" t="s">
         <v>129</v>
-      </c>
-      <c r="H3" s="28" t="s">
-        <v>130</v>
       </c>
     </row>
     <row r="4" ht="14.25" customHeight="1">
       <c r="A4" s="28" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="B4" s="28" t="s">
+        <v>130</v>
+      </c>
+      <c r="C4" s="41" t="s">
         <v>131</v>
       </c>
-      <c r="C4" s="40" t="s">
+      <c r="D4" s="42" t="s">
         <v>132</v>
       </c>
-      <c r="D4" s="41" t="s">
+      <c r="E4" s="28" t="s">
         <v>133</v>
       </c>
-      <c r="E4" s="28" t="s">
+      <c r="F4" s="41" t="s">
         <v>134</v>
       </c>
-      <c r="F4" s="40" t="s">
-        <v>135</v>
-      </c>
       <c r="H4" s="28" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
     </row>
     <row r="5" ht="14.25" customHeight="1">

</xml_diff>